<commit_message>
updated timeline, code cleanup for login/signup done
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_18_Mar.xlsx
+++ b/other/Project_TimeLine_2021_18_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9080AA-9897-4A0A-8375-1BAAB9EB82BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4CE90B6-3B74-4FA6-B81C-90D8BA83D58E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="36">
   <si>
     <t>S/N</t>
   </si>
@@ -135,10 +135,14 @@
     <t>Front-end: Data charts</t>
   </si>
   <si>
-    <t>Re-estimated start/finish</t>
-  </si>
-  <si>
-    <t>Have to clarify with Viola on the layout of this page</t>
+    <t>Front-end: Relocation pop-up</t>
+  </si>
+  <si>
+    <t>Code refactoring</t>
+  </si>
+  <si>
+    <t>Code is becoming really
+messy (especially CSS). Would have to clean up for better scalability.</t>
   </si>
 </sst>
 </file>
@@ -519,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -892,7 +896,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -914,9 +918,7 @@
       <c r="G16" s="3">
         <v>44265</v>
       </c>
-      <c r="I16" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="I16" s="4"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -937,64 +939,77 @@
       <c r="F17" s="3">
         <v>44272</v>
       </c>
-      <c r="H17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="G17" s="3">
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>44271</v>
+      </c>
+      <c r="F18" s="3">
+        <v>44272</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18">
-        <v>5</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="I18" s="4" t="s">
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="I22" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>15</v>
       </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19">
-        <v>2</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="H19" t="s">
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="H23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="H20" t="s">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="H24" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>